<commit_message>
re-export experiment results with better table structure
</commit_message>
<xml_diff>
--- a/result_exporter/Result_CyclicABP_Iteration_Symmetry_Highest_1800s.xlsx
+++ b/result_exporter/Result_CyclicABP_Iteration_Symmetry_Highest_1800s.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="11">
   <si>
     <t>Width</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>UNSAT</t>
+  </si>
+  <si>
+    <t>Max width SAT</t>
+  </si>
+  <si>
+    <t>Min width UNSAT</t>
+  </si>
+  <si>
+    <t>Total real time (s)</t>
+  </si>
+  <si>
+    <t>Total memory consumed (MB)</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -412,13 +427,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,8 +446,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>3</v>
       </c>
@@ -445,8 +466,14 @@
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>4</v>
       </c>
@@ -459,8 +486,14 @@
       <c r="D3">
         <v>0.001</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>0.383</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>5</v>
       </c>
@@ -473,8 +506,14 @@
       <c r="D4">
         <v>0.029</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>6</v>
       </c>
@@ -488,7 +527,7 @@
         <v>0.003</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>7</v>
       </c>
@@ -509,13 +548,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,8 +567,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>16</v>
       </c>
@@ -542,8 +587,14 @@
       <c r="D2">
         <v>0.032</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>17</v>
       </c>
@@ -556,8 +607,14 @@
       <c r="D3">
         <v>0.028</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>19.823</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>18</v>
       </c>
@@ -570,8 +627,14 @@
       <c r="D4">
         <v>0.028</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>78.09999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>19</v>
       </c>
@@ -585,7 +648,7 @@
         <v>0.024</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>20</v>
       </c>
@@ -599,7 +662,7 @@
         <v>0.026</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>21</v>
       </c>
@@ -613,7 +676,7 @@
         <v>0.025</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>22</v>
       </c>
@@ -627,7 +690,7 @@
         <v>0.029</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>23</v>
       </c>
@@ -641,7 +704,7 @@
         <v>0.193</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>24</v>
       </c>
@@ -655,7 +718,7 @@
         <v>2.534</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>25</v>
       </c>
@@ -669,7 +732,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>26</v>
       </c>
@@ -683,7 +746,7 @@
         <v>0.274</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>27</v>
       </c>
@@ -697,7 +760,7 @@
         <v>0.298</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>28</v>
       </c>
@@ -711,7 +774,7 @@
         <v>0.243</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>29</v>
       </c>
@@ -725,7 +788,7 @@
         <v>1.441</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>30</v>
       </c>
@@ -788,13 +851,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -807,8 +870,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>23</v>
       </c>
@@ -821,8 +890,14 @@
       <c r="D2">
         <v>0.261</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>24</v>
       </c>
@@ -835,8 +910,14 @@
       <c r="D3">
         <v>0.163</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1806.026</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>25</v>
       </c>
@@ -849,8 +930,14 @@
       <c r="D4">
         <v>0.215</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>355.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>26</v>
       </c>
@@ -864,7 +951,7 @@
         <v>0.282</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>27</v>
       </c>
@@ -878,7 +965,7 @@
         <v>0.411</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>28</v>
       </c>
@@ -892,7 +979,7 @@
         <v>0.282</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>29</v>
       </c>
@@ -906,7 +993,7 @@
         <v>1.146</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>30</v>
       </c>
@@ -920,7 +1007,7 @@
         <v>0.091</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>31</v>
       </c>
@@ -934,7 +1021,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>32</v>
       </c>
@@ -948,7 +1035,7 @@
         <v>1.643</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>33</v>
       </c>
@@ -962,7 +1049,7 @@
         <v>2.176</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>34</v>
       </c>
@@ -976,7 +1063,7 @@
         <v>1.439</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>35</v>
       </c>
@@ -990,7 +1077,7 @@
         <v>1.985</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>36</v>
       </c>
@@ -1004,7 +1091,7 @@
         <v>1.907</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>37</v>
       </c>
@@ -1151,13 +1238,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1170,8 +1257,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>20</v>
       </c>
@@ -1184,8 +1277,14 @@
       <c r="D2">
         <v>0.038</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>21</v>
       </c>
@@ -1198,8 +1297,14 @@
       <c r="D3">
         <v>0.041</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>3.919</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>22</v>
       </c>
@@ -1212,8 +1317,14 @@
       <c r="D4">
         <v>0.038</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>71.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>23</v>
       </c>
@@ -1227,7 +1338,7 @@
         <v>0.045</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>24</v>
       </c>
@@ -1241,7 +1352,7 @@
         <v>0.033</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>25</v>
       </c>
@@ -1255,7 +1366,7 @@
         <v>0.043</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>26</v>
       </c>
@@ -1269,7 +1380,7 @@
         <v>0.045</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>27</v>
       </c>
@@ -1283,7 +1394,7 @@
         <v>1.594</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>28</v>
       </c>
@@ -1297,7 +1408,7 @@
         <v>0.412</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>29</v>
       </c>
@@ -1311,7 +1422,7 @@
         <v>0.035</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>30</v>
       </c>
@@ -1332,13 +1443,13 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1351,8 +1462,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>14</v>
       </c>
@@ -1365,8 +1482,14 @@
       <c r="D2">
         <v>1.568</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>15</v>
       </c>
@@ -1379,8 +1502,14 @@
       <c r="D3">
         <v>1.527</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1806.108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>16</v>
       </c>
@@ -1393,8 +1522,14 @@
       <c r="D4">
         <v>1.879</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>2078.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>17</v>
       </c>
@@ -1408,7 +1543,7 @@
         <v>13.024</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>18</v>
       </c>
@@ -1422,7 +1557,7 @@
         <v>1.762</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>19</v>
       </c>
@@ -1436,7 +1571,7 @@
         <v>1.794</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>20</v>
       </c>
@@ -1450,7 +1585,7 @@
         <v>1.532</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>21</v>
       </c>
@@ -1464,7 +1599,7 @@
         <v>1.848</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>22</v>
       </c>
@@ -1478,7 +1613,7 @@
         <v>1.831</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>23</v>
       </c>
@@ -1492,7 +1627,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>24</v>
       </c>
@@ -1506,7 +1641,7 @@
         <v>1.862</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>25</v>
       </c>
@@ -1520,7 +1655,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>26</v>
       </c>
@@ -1534,7 +1669,7 @@
         <v>4.694</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>27</v>
       </c>
@@ -1548,7 +1683,7 @@
         <v>50.6</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>28</v>
       </c>
@@ -1639,13 +1774,13 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1658,8 +1793,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>14</v>
       </c>
@@ -1672,8 +1813,14 @@
       <c r="D2">
         <v>1.404</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>15</v>
       </c>
@@ -1686,8 +1833,14 @@
       <c r="D3">
         <v>1.451</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1806.013</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>16</v>
       </c>
@@ -1700,8 +1853,14 @@
       <c r="D4">
         <v>1.705</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>2075.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>17</v>
       </c>
@@ -1715,7 +1874,7 @@
         <v>12.175</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>18</v>
       </c>
@@ -1729,7 +1888,7 @@
         <v>1.604</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>19</v>
       </c>
@@ -1743,7 +1902,7 @@
         <v>1.742</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>20</v>
       </c>
@@ -1757,7 +1916,7 @@
         <v>1.484</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>21</v>
       </c>
@@ -1771,7 +1930,7 @@
         <v>1.688</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>22</v>
       </c>
@@ -1785,7 +1944,7 @@
         <v>1.787</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>23</v>
       </c>
@@ -1799,7 +1958,7 @@
         <v>1.407</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>24</v>
       </c>
@@ -1813,7 +1972,7 @@
         <v>1.837</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>25</v>
       </c>
@@ -1827,7 +1986,7 @@
         <v>1.846</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>26</v>
       </c>
@@ -1841,7 +2000,7 @@
         <v>4.588</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>27</v>
       </c>
@@ -1855,7 +2014,7 @@
         <v>47.679</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>28</v>
       </c>
@@ -1946,13 +2105,13 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1965,8 +2124,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>46</v>
       </c>
@@ -1979,8 +2144,14 @@
       <c r="D2">
         <v>0.667</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>47</v>
       </c>
@@ -1993,8 +2164,14 @@
       <c r="D3">
         <v>0.66</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1805.881</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>48</v>
       </c>
@@ -2007,8 +2184,14 @@
       <c r="D4">
         <v>0.597</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>49</v>
       </c>
@@ -2022,7 +2205,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>50</v>
       </c>
@@ -2036,7 +2219,7 @@
         <v>0.617</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>51</v>
       </c>
@@ -2050,7 +2233,7 @@
         <v>0.654</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>52</v>
       </c>
@@ -2064,7 +2247,7 @@
         <v>28.175</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>53</v>
       </c>
@@ -2078,7 +2261,7 @@
         <v>0.583</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>54</v>
       </c>
@@ -2092,7 +2275,7 @@
         <v>0.602</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>55</v>
       </c>
@@ -2106,7 +2289,7 @@
         <v>0.614</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>56</v>
       </c>
@@ -2120,7 +2303,7 @@
         <v>53.216</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>57</v>
       </c>
@@ -2134,7 +2317,7 @@
         <v>1.522</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>58</v>
       </c>
@@ -2148,7 +2331,7 @@
         <v>1.137</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>59</v>
       </c>
@@ -2162,7 +2345,7 @@
         <v>20.238</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>60</v>
       </c>
@@ -2589,13 +2772,13 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2608,8 +2791,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>39</v>
       </c>
@@ -2622,8 +2811,14 @@
       <c r="D2">
         <v>3.427</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>40</v>
       </c>
@@ -2636,8 +2831,14 @@
       <c r="D3">
         <v>0.706</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1806.029</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>41</v>
       </c>
@@ -2650,8 +2851,14 @@
       <c r="D4">
         <v>0.6919999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>1444.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>42</v>
       </c>
@@ -2665,7 +2872,7 @@
         <v>6.014</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>43</v>
       </c>
@@ -2679,7 +2886,7 @@
         <v>4.357</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>44</v>
       </c>
@@ -2693,7 +2900,7 @@
         <v>0.6879999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>45</v>
       </c>
@@ -2707,7 +2914,7 @@
         <v>23.665</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>46</v>
       </c>
@@ -2721,7 +2928,7 @@
         <v>0.704</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>47</v>
       </c>
@@ -2735,7 +2942,7 @@
         <v>57.542</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>48</v>
       </c>
@@ -2749,7 +2956,7 @@
         <v>22.089</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>49</v>
       </c>
@@ -2763,7 +2970,7 @@
         <v>0.742</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>50</v>
       </c>
@@ -2777,7 +2984,7 @@
         <v>0.673</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>51</v>
       </c>
@@ -2791,7 +2998,7 @@
         <v>54.401</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>52</v>
       </c>
@@ -2805,7 +3012,7 @@
         <v>65.45999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>53</v>
       </c>
@@ -3022,13 +3229,13 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3041,8 +3248,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>110</v>
       </c>
@@ -3055,8 +3268,14 @@
       <c r="D2">
         <v>27.557</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>111</v>
       </c>
@@ -3069,8 +3288,14 @@
       <c r="D3">
         <v>47.633</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1806.722</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>112</v>
       </c>
@@ -3083,8 +3308,14 @@
       <c r="D4">
         <v>84.667</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>1257.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>113</v>
       </c>
@@ -3098,7 +3329,7 @@
         <v>63.355</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>114</v>
       </c>
@@ -3112,7 +3343,7 @@
         <v>88.00700000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>115</v>
       </c>
@@ -3126,7 +3357,7 @@
         <v>31.403</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>116</v>
       </c>
@@ -3140,7 +3371,7 @@
         <v>29.904</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>117</v>
       </c>
@@ -3154,7 +3385,7 @@
         <v>18.386</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>118</v>
       </c>
@@ -3168,7 +3399,7 @@
         <v>66.789</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>119</v>
       </c>
@@ -3182,7 +3413,7 @@
         <v>1.689</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>120</v>
       </c>
@@ -3196,7 +3427,7 @@
         <v>33.337</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>121</v>
       </c>
@@ -3210,7 +3441,7 @@
         <v>26.505</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>122</v>
       </c>
@@ -3224,7 +3455,7 @@
         <v>28.352</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>123</v>
       </c>
@@ -3238,7 +3469,7 @@
         <v>91.709</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>124</v>
       </c>
@@ -3441,13 +3672,13 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3460,8 +3691,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>23</v>
       </c>
@@ -3474,8 +3711,14 @@
       <c r="D2">
         <v>0.9370000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>24</v>
       </c>
@@ -3488,8 +3731,14 @@
       <c r="D3">
         <v>0.876</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1806.459</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>25</v>
       </c>
@@ -3502,8 +3751,14 @@
       <c r="D4">
         <v>0.876</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>2157.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>26</v>
       </c>
@@ -3517,7 +3772,7 @@
         <v>0.9360000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>27</v>
       </c>
@@ -3531,7 +3786,7 @@
         <v>0.945</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>28</v>
       </c>
@@ -3545,7 +3800,7 @@
         <v>0.9330000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>29</v>
       </c>
@@ -3559,7 +3814,7 @@
         <v>65.372</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>30</v>
       </c>
@@ -3573,7 +3828,7 @@
         <v>0.913</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>31</v>
       </c>
@@ -3587,7 +3842,7 @@
         <v>2.54</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>32</v>
       </c>
@@ -3601,7 +3856,7 @@
         <v>2.015</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>33</v>
       </c>
@@ -3615,7 +3870,7 @@
         <v>2.587</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>34</v>
       </c>
@@ -3629,7 +3884,7 @@
         <v>1.985</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>35</v>
       </c>
@@ -3643,7 +3898,7 @@
         <v>2.579</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>36</v>
       </c>
@@ -3657,7 +3912,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>37</v>
       </c>
@@ -4000,13 +4255,13 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4019,8 +4274,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>128</v>
       </c>
@@ -4033,8 +4294,14 @@
       <c r="D2">
         <v>148.746</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>129</v>
       </c>
@@ -4047,8 +4314,14 @@
       <c r="D3">
         <v>157.985</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1806.561</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>130</v>
       </c>
@@ -4061,8 +4334,14 @@
       <c r="D4">
         <v>135.346</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>1703.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>131</v>
       </c>
@@ -4076,7 +4355,7 @@
         <v>154.819</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>132</v>
       </c>
@@ -4090,7 +4369,7 @@
         <v>142.269</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>133</v>
       </c>
@@ -4104,7 +4383,7 @@
         <v>172.519</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>134</v>
       </c>
@@ -4118,7 +4397,7 @@
         <v>160.46</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>135</v>
       </c>
@@ -4132,7 +4411,7 @@
         <v>193.992</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>136</v>
       </c>
@@ -4146,7 +4425,7 @@
         <v>137.205</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>137</v>
       </c>
@@ -4160,7 +4439,7 @@
         <v>159.225</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>138</v>
       </c>
@@ -4181,13 +4460,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4200,8 +4479,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>5</v>
       </c>
@@ -4214,8 +4499,14 @@
       <c r="D2">
         <v>0.001</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>6</v>
       </c>
@@ -4228,8 +4519,14 @@
       <c r="D3">
         <v>0.002</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>0.096</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>7</v>
       </c>
@@ -4242,8 +4539,14 @@
       <c r="D4">
         <v>0.002</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>8</v>
       </c>
@@ -4257,7 +4560,7 @@
         <v>0.016</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>9</v>
       </c>
@@ -4278,13 +4581,13 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4297,8 +4600,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>52</v>
       </c>
@@ -4311,8 +4620,14 @@
       <c r="D2">
         <v>1.204</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>53</v>
       </c>
@@ -4325,8 +4640,14 @@
       <c r="D3">
         <v>73.18600000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1805.728</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>54</v>
       </c>
@@ -4339,8 +4660,14 @@
       <c r="D4">
         <v>15.676</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>2545.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>55</v>
       </c>
@@ -4354,7 +4681,7 @@
         <v>2.121</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>56</v>
       </c>
@@ -4368,7 +4695,7 @@
         <v>126.781</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>57</v>
       </c>
@@ -4382,7 +4709,7 @@
         <v>83.809</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>58</v>
       </c>
@@ -4396,7 +4723,7 @@
         <v>1.167</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>59</v>
       </c>
@@ -4410,7 +4737,7 @@
         <v>85.15300000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>60</v>
       </c>
@@ -4424,7 +4751,7 @@
         <v>3.32</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>61</v>
       </c>
@@ -4438,7 +4765,7 @@
         <v>110.175</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>62</v>
       </c>
@@ -4452,7 +4779,7 @@
         <v>107.205</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>63</v>
       </c>
@@ -4466,7 +4793,7 @@
         <v>231.289</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>64</v>
       </c>
@@ -4480,7 +4807,7 @@
         <v>2.175</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>65</v>
       </c>
@@ -4494,7 +4821,7 @@
         <v>38.535</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>66</v>
       </c>
@@ -4641,13 +4968,13 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4660,8 +4987,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>110</v>
       </c>
@@ -4674,8 +5007,14 @@
       <c r="D2">
         <v>94.34</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>111</v>
       </c>
@@ -4688,8 +5027,14 @@
       <c r="D3">
         <v>34.801</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1805.805</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>112</v>
       </c>
@@ -4702,8 +5047,14 @@
       <c r="D4">
         <v>37.912</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>2150.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>113</v>
       </c>
@@ -4717,7 +5068,7 @@
         <v>41.2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>114</v>
       </c>
@@ -4731,7 +5082,7 @@
         <v>35.246</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>115</v>
       </c>
@@ -4745,7 +5096,7 @@
         <v>6.064</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>116</v>
       </c>
@@ -4759,7 +5110,7 @@
         <v>93.902</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>117</v>
       </c>
@@ -4773,7 +5124,7 @@
         <v>103.579</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>118</v>
       </c>
@@ -4787,7 +5138,7 @@
         <v>70.435</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>119</v>
       </c>
@@ -4801,7 +5152,7 @@
         <v>107.799</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>120</v>
       </c>
@@ -4815,7 +5166,7 @@
         <v>117.036</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>121</v>
       </c>
@@ -4829,7 +5180,7 @@
         <v>8.414</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>122</v>
       </c>
@@ -4843,7 +5194,7 @@
         <v>78.69499999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>123</v>
       </c>
@@ -4857,7 +5208,7 @@
         <v>100.829</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>124</v>
       </c>
@@ -5060,13 +5411,13 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5079,8 +5430,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>163</v>
       </c>
@@ -5093,8 +5450,14 @@
       <c r="D2">
         <v>122.425</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>164</v>
       </c>
@@ -5107,8 +5470,14 @@
       <c r="D3">
         <v>170.233</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1805.788</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>165</v>
       </c>
@@ -5121,8 +5490,14 @@
       <c r="D4">
         <v>221.748</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>2531.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>166</v>
       </c>
@@ -5136,7 +5511,7 @@
         <v>251.625</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>167</v>
       </c>
@@ -5150,7 +5525,7 @@
         <v>159.96</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>168</v>
       </c>
@@ -5164,7 +5539,7 @@
         <v>132.295</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>169</v>
       </c>
@@ -5178,7 +5553,7 @@
         <v>197.726</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>170</v>
       </c>
@@ -5199,13 +5574,13 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5218,8 +5593,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>68</v>
       </c>
@@ -5232,8 +5613,14 @@
       <c r="D2">
         <v>40.286</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>69</v>
       </c>
@@ -5246,8 +5633,14 @@
       <c r="D3">
         <v>1.526</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1805.679</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>70</v>
       </c>
@@ -5260,8 +5653,14 @@
       <c r="D4">
         <v>1.513</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>2508.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>71</v>
       </c>
@@ -5275,7 +5674,7 @@
         <v>1.577</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>72</v>
       </c>
@@ -5289,7 +5688,7 @@
         <v>1.564</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>73</v>
       </c>
@@ -5303,7 +5702,7 @@
         <v>8.146000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>74</v>
       </c>
@@ -5317,7 +5716,7 @@
         <v>1.559</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>75</v>
       </c>
@@ -5331,7 +5730,7 @@
         <v>2.762</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>76</v>
       </c>
@@ -5345,7 +5744,7 @@
         <v>3.368</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>77</v>
       </c>
@@ -5359,7 +5758,7 @@
         <v>1.371</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>78</v>
       </c>
@@ -5373,7 +5772,7 @@
         <v>2.338</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>79</v>
       </c>
@@ -5387,7 +5786,7 @@
         <v>1.344</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>80</v>
       </c>
@@ -5401,7 +5800,7 @@
         <v>1.382</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>81</v>
       </c>
@@ -5415,7 +5814,7 @@
         <v>3.332</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>82</v>
       </c>
@@ -5842,13 +6241,13 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5861,8 +6260,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>56</v>
       </c>
@@ -5875,8 +6280,14 @@
       <c r="D2">
         <v>8.253</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>57</v>
       </c>
@@ -5889,8 +6300,14 @@
       <c r="D3">
         <v>3.397</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1805.695</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>58</v>
       </c>
@@ -5903,8 +6320,14 @@
       <c r="D4">
         <v>3.355</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>3634.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>59</v>
       </c>
@@ -5918,7 +6341,7 @@
         <v>168.154</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>60</v>
       </c>
@@ -5932,7 +6355,7 @@
         <v>9.422000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>61</v>
       </c>
@@ -5946,7 +6369,7 @@
         <v>81.033</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>62</v>
       </c>
@@ -5960,7 +6383,7 @@
         <v>165.116</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>63</v>
       </c>
@@ -5974,7 +6397,7 @@
         <v>134.091</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>64</v>
       </c>
@@ -5988,7 +6411,7 @@
         <v>148.612</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>65</v>
       </c>
@@ -6002,7 +6425,7 @@
         <v>140.308</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>66</v>
       </c>
@@ -6016,7 +6439,7 @@
         <v>52.979</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>67</v>
       </c>
@@ -6030,7 +6453,7 @@
         <v>10.857</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>68</v>
       </c>
@@ -6044,7 +6467,7 @@
         <v>25.997</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>69</v>
       </c>
@@ -6058,7 +6481,7 @@
         <v>226.504</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>70</v>
       </c>
@@ -6121,13 +6544,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6140,8 +6563,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>8</v>
       </c>
@@ -6154,8 +6583,14 @@
       <c r="D2">
         <v>0.002</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>9</v>
       </c>
@@ -6168,8 +6603,14 @@
       <c r="D3">
         <v>0.003</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>0.177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>10</v>
       </c>
@@ -6182,8 +6623,14 @@
       <c r="D4">
         <v>0.002</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>11</v>
       </c>
@@ -6197,7 +6644,7 @@
         <v>0.002</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>12</v>
       </c>
@@ -6211,7 +6658,7 @@
         <v>0.032</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>13</v>
       </c>
@@ -6225,7 +6672,7 @@
         <v>0.035</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>14</v>
       </c>
@@ -6246,13 +6693,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6265,8 +6712,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>4</v>
       </c>
@@ -6279,8 +6732,14 @@
       <c r="D2">
         <v>0.003</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>5</v>
       </c>
@@ -6293,8 +6752,14 @@
       <c r="D3">
         <v>0.005</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>0.289</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>6</v>
       </c>
@@ -6307,8 +6772,14 @@
       <c r="D4">
         <v>0.006</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>16.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>7</v>
       </c>
@@ -6322,7 +6793,7 @@
         <v>0.004</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>8</v>
       </c>
@@ -6336,7 +6807,7 @@
         <v>0.023</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>9</v>
       </c>
@@ -6357,13 +6828,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6376,8 +6847,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>11</v>
       </c>
@@ -6390,8 +6867,14 @@
       <c r="D2">
         <v>0.005</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>12</v>
       </c>
@@ -6404,8 +6887,14 @@
       <c r="D3">
         <v>0.004</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>0.182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>13</v>
       </c>
@@ -6418,8 +6907,14 @@
       <c r="D4">
         <v>0.004</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>14</v>
       </c>
@@ -6433,7 +6928,7 @@
         <v>0.005</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>15</v>
       </c>
@@ -6447,7 +6942,7 @@
         <v>0.007</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>16</v>
       </c>
@@ -6461,7 +6956,7 @@
         <v>0.005</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>17</v>
       </c>
@@ -6482,13 +6977,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6501,8 +6996,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>6</v>
       </c>
@@ -6515,8 +7016,14 @@
       <c r="D2">
         <v>0.004</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>7</v>
       </c>
@@ -6529,8 +7036,14 @@
       <c r="D3">
         <v>0.005</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>0.213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>8</v>
       </c>
@@ -6543,8 +7056,14 @@
       <c r="D4">
         <v>0.006</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>17.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>9</v>
       </c>
@@ -6558,7 +7077,7 @@
         <v>0.004</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>10</v>
       </c>
@@ -6572,7 +7091,7 @@
         <v>0.014</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>11</v>
       </c>
@@ -6593,13 +7112,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6612,8 +7131,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>6</v>
       </c>
@@ -6626,8 +7151,14 @@
       <c r="D2">
         <v>0.006</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>7</v>
       </c>
@@ -6640,8 +7171,14 @@
       <c r="D3">
         <v>0.005</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>0.363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>8</v>
       </c>
@@ -6654,8 +7191,14 @@
       <c r="D4">
         <v>0.005</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>19.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>9</v>
       </c>
@@ -6669,7 +7212,7 @@
         <v>0.005</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>10</v>
       </c>
@@ -6683,7 +7226,7 @@
         <v>0.066</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>11</v>
       </c>
@@ -6697,7 +7240,7 @@
         <v>0.035</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>12</v>
       </c>
@@ -6718,13 +7261,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6737,8 +7280,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>4</v>
       </c>
@@ -6751,8 +7300,14 @@
       <c r="D2">
         <v>0.003</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>5</v>
       </c>
@@ -6765,8 +7320,14 @@
       <c r="D3">
         <v>0.005</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>2.557</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>6</v>
       </c>
@@ -6779,8 +7340,14 @@
       <c r="D4">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>7</v>
       </c>
@@ -6794,7 +7361,7 @@
         <v>0.077</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>8</v>
       </c>
@@ -6815,13 +7382,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6834,8 +7401,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>10</v>
       </c>
@@ -6848,8 +7421,14 @@
       <c r="D2">
         <v>0.015</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>11</v>
       </c>
@@ -6862,8 +7441,14 @@
       <c r="D3">
         <v>0.016</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>3.598</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>12</v>
       </c>
@@ -6876,8 +7461,14 @@
       <c r="D4">
         <v>0.015</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>13</v>
       </c>
@@ -6891,7 +7482,7 @@
         <v>0.014</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>14</v>
       </c>
@@ -6905,7 +7496,7 @@
         <v>0.015</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>15</v>
       </c>
@@ -6919,7 +7510,7 @@
         <v>0.015</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>16</v>
       </c>
@@ -6933,7 +7524,7 @@
         <v>0.018</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>17</v>
       </c>
@@ -6947,7 +7538,7 @@
         <v>0.017</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>18</v>
       </c>
@@ -6961,7 +7552,7 @@
         <v>0.026</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>19</v>
       </c>
@@ -6975,7 +7566,7 @@
         <v>0.055</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>20</v>
       </c>
@@ -6989,7 +7580,7 @@
         <v>0.244</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>21</v>
       </c>
@@ -7003,7 +7594,7 @@
         <v>2.034</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>22</v>
       </c>

</xml_diff>